<commit_message>
add tree chart example to excel
</commit_message>
<xml_diff>
--- a/problems.xlsx
+++ b/problems.xlsx
@@ -8,17 +8,56 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob.jahn/dev/dt-demos/problem-report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9998CF2A-FD06-434A-BA43-1093932C869A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86451E3-C0A2-A44B-B1F5-16FB3AD498A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2080" yWindow="2340" windowWidth="24720" windowHeight="15900" activeTab="1" xr2:uid="{670C6F68-BB05-854A-BFF1-35C4E762D949}"/>
+    <workbookView xWindow="2080" yWindow="2340" windowWidth="24720" windowHeight="15900" activeTab="2" xr2:uid="{670C6F68-BB05-854A-BFF1-35C4E762D949}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
-    <sheet name="chart" sheetId="2" r:id="rId2"/>
+    <sheet name="line chart" sheetId="2" r:id="rId2"/>
+    <sheet name="tree chart" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'line chart'!$I$22</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'line chart'!$I$22</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">'line chart'!$A$5:$A$8</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">'line chart'!$B$4</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">'line chart'!$B$5:$B$8</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">'line chart'!$C$4</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">'line chart'!$C$5:$C$8</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">'line chart'!$D$4</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">'line chart'!$D$5:$D$8</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">'line chart'!$I$22</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">'tree chart'!$A$4:$A$5</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">'tree chart'!$A$5:$A$8</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'line chart'!$A$5:$A$8</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">'tree chart'!$B$4</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">'tree chart'!$B$4:$B$5</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">'tree chart'!$B$5:$B$8</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">'tree chart'!$C$4</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">'tree chart'!$C$5:$C$8</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">'tree chart'!$D$4</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">'tree chart'!$D$5:$D$8</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">'tree chart'!$A$4:$A$5</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">'tree chart'!$A$5:$A$8</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">'tree chart'!$B$4</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'line chart'!$B$4</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">'tree chart'!$B$4:$B$5</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">'tree chart'!$B$5:$B$8</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">'tree chart'!$C$4</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">'tree chart'!$C$5:$C$8</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">'tree chart'!$D$4</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">'tree chart'!$D$5:$D$8</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'line chart'!$B$5:$B$8</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'line chart'!$C$4</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'line chart'!$C$5:$C$8</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'line chart'!$D$4</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'line chart'!$D$5:$D$8</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'line chart'!$I$22</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="13" r:id="rId3"/>
+    <pivotCache cacheId="15" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="39">
   <si>
     <t>problem</t>
   </si>
@@ -241,7 +280,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[problem.xlsx]chart!PivotTable2</c:name>
+    <c:name>[problems.xlsx]line chart!PivotTable2</c:name>
     <c:fmtId val="1"/>
   </c:pivotSource>
   <c:chart>
@@ -318,6 +357,9 @@
       <c:pivotFmt>
         <c:idx val="1"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -460,7 +502,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>chart!$B$3:$B$4</c:f>
+              <c:f>'line chart'!$B$3:$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -495,7 +537,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>chart!$A$5:$A$9</c:f>
+              <c:f>'line chart'!$A$5:$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -515,7 +557,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>chart!$B$5:$B$9</c:f>
+              <c:f>'line chart'!$B$5:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -546,7 +588,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>chart!$C$3:$C$4</c:f>
+              <c:f>'line chart'!$C$3:$C$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -581,7 +623,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>chart!$A$5:$A$9</c:f>
+              <c:f>'line chart'!$A$5:$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -601,7 +643,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>chart!$C$5:$C$9</c:f>
+              <c:f>'line chart'!$C$5:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -840,7 +882,73 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.27</cx:f>
+      </cx:strDim>
+      <cx:numDim type="size">
+        <cx:f>_xlchart.v1.30</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="treemap" uniqueId="{B9BC2A02-5648-9841-ABFF-CAE9E41DE02F}">
+          <cx:dataId val="0"/>
+          <cx:layoutPr/>
+        </cx:series>
+      </cx:plotAreaRegion>
+    </cx:plotArea>
+    <cx:legend pos="r" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1383,6 +1491,528 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="410">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1">
+          <a:lumMod val="65000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1419,6 +2049,89 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>273050</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>527050</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>196850</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Chart 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CA56BA4-4104-744E-865D-820B7953C43E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4616450" y="908050"/>
+              <a:ext cx="4381500" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1593,7 +2306,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CF2F407F-8AC5-1B4B-8792-CC16A5631BD0}" name="PivotTable2" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CF2F407F-8AC5-1B4B-8792-CC16A5631BD0}" name="PivotTable2" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
   <location ref="A3:D9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField dataField="1" showAll="0"/>
@@ -1657,7 +2370,7 @@
   <dataFields count="1">
     <dataField name="Count of problem" fld="0" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="5">
+  <chartFormats count="9">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -1711,6 +2424,239 @@
           </reference>
           <reference field="4" count="1" selected="0">
             <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="6" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0EBE852B-3132-F64A-A2A4-9549D6CB2A25}" name="PivotTable2" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
+  <location ref="A3:B6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item h="1" x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of problem" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="11">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="6" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
           </reference>
         </references>
       </pivotArea>
@@ -2345,8 +3291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{195E2901-D06B-844D-9422-5339FC90E781}">
   <dimension ref="A3:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2383,11 +3329,10 @@
       <c r="A5" s="4">
         <v>44962</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6">
+      <c r="D5">
         <v>1</v>
       </c>
     </row>
@@ -2395,11 +3340,10 @@
       <c r="A6" s="4">
         <v>44963</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6">
+      <c r="D6">
         <v>2</v>
       </c>
     </row>
@@ -2407,13 +3351,13 @@
       <c r="A7" s="4">
         <v>44964</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7">
         <v>4</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7">
         <v>2</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7">
         <v>6</v>
       </c>
     </row>
@@ -2421,13 +3365,13 @@
       <c r="A8" s="4">
         <v>44965</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8">
         <v>2</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8">
         <v>1</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8">
         <v>3</v>
       </c>
     </row>
@@ -2435,13 +3379,67 @@
       <c r="A9" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9">
         <v>9</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9">
         <v>3</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{557993E5-FA8B-0742-9144-7097181924C1}">
+  <dimension ref="A3:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="6">
         <v>12</v>
       </c>
     </row>

</xml_diff>